<commit_message>
thêm trang web + hiệu chỉnh sql
</commit_message>
<xml_diff>
--- a/du lieu sach.xlsx
+++ b/du lieu sach.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\hk6\DATN\DATN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HK6\DATN\DATN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE60D419-C441-4FA4-AECA-1CD08CFADF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6C3155-5247-477F-9840-5A8C2C31AB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="8145" windowWidth="14340" windowHeight="8055" tabRatio="611" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="268">
   <si>
     <t>MaSach</t>
   </si>
@@ -1200,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="E120" sqref="E120"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,7 +1215,7 @@
     <col min="9" max="9" width="8.42578125" style="2" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="19.140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="2" customWidth="1"/>
     <col min="13" max="13" width="168.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1286,8 +1286,8 @@
       <c r="I2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>192</v>
+      <c r="J2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K2" s="3">
         <v>44993.412780362698</v>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="M2" t="str">
         <f>"INSERT INTO Sach VALUES('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"',"&amp;D2&amp;",N'"&amp;E2&amp;"',"&amp;F2&amp;",'"&amp;G2&amp;"',"&amp;H2&amp;",1,"&amp;J2&amp;",'',"&amp;L2&amp;")"</f>
-        <v>INSERT INTO Sach VALUES('nv61','GD','GK',NULL,N'Ngữ văn lớp 6 tập 1',NULL,'nv61.jpg',6000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('nv61','GD','GK',NULL,N'Ngữ văn lớp 6 tập 1',NULL,'nv61.jpg',6000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1329,8 +1329,8 @@
       <c r="I3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>192</v>
+      <c r="J3" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K3" s="3">
         <v>44993.412780362698</v>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="M3" t="str">
         <f t="shared" ref="M3:M66" si="1">"INSERT INTO Sach VALUES('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"',"&amp;D3&amp;",N'"&amp;E3&amp;"',"&amp;F3&amp;",'"&amp;G3&amp;"',"&amp;H3&amp;",1,"&amp;J3&amp;",'',"&amp;L3&amp;")"</f>
-        <v>INSERT INTO Sach VALUES('nv62','GD','GK',NULL,N'Ngữ văn 6 lớp tập 2',NULL,'nv62.jpg',6000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('nv62','GD','GK',NULL,N'Ngữ văn 6 lớp tập 2',NULL,'nv62.jpg',6000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1372,8 +1372,8 @@
       <c r="I4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>192</v>
+      <c r="J4" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K4" s="3">
         <v>44993.412780362698</v>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="M4" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('nv71','GD','GK',NULL,N'Ngữ văn lớp 7 tập 1',NULL,'nv71.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('nv71','GD','GK',NULL,N'Ngữ văn lớp 7 tập 1',NULL,'nv71.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1415,8 +1415,8 @@
       <c r="I5" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>192</v>
+      <c r="J5" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K5" s="3">
         <v>44993.412780362698</v>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="M5" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('nv72','GD','GK',NULL,N'Ngữ văn lớp 7 tập 2',NULL,'nv72.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('nv72','GD','GK',NULL,N'Ngữ văn lớp 7 tập 2',NULL,'nv72.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1458,8 +1458,8 @@
       <c r="I6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>192</v>
+      <c r="J6" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K6" s="3">
         <v>44993.412780362698</v>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="M6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('nv81','GD','GK',NULL,N'Ngữ văn lớp 8 tập 1',NULL,'nv81.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('nv81','GD','GK',NULL,N'Ngữ văn lớp 8 tập 1',NULL,'nv81.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1501,8 +1501,8 @@
       <c r="I7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>192</v>
+      <c r="J7" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K7" s="3">
         <v>44993.412780362698</v>
@@ -1512,7 +1512,7 @@
       </c>
       <c r="M7" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('nv82','GD','GK',NULL,N'Ngữ văn lớp 8 tập 2',NULL,'nv82.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('nv82','GD','GK',NULL,N'Ngữ văn lớp 8 tập 2',NULL,'nv82.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1544,8 +1544,8 @@
       <c r="I8" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>192</v>
+      <c r="J8" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K8" s="3">
         <v>44993.412780362698</v>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="M8" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('nv91','GD','GK',NULL,N'Ngữ văn lớp 9 tập 1',NULL,'nv91.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('nv91','GD','GK',NULL,N'Ngữ văn lớp 9 tập 1',NULL,'nv91.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1587,8 +1587,8 @@
       <c r="I9" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>192</v>
+      <c r="J9" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K9" s="3">
         <v>44993.412780362698</v>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="M9" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('nv92','GD','GK',NULL,N'Ngữ văn lớp 9 tập 2',NULL,'nv92.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('nv92','GD','GK',NULL,N'Ngữ văn lớp 9 tập 2',NULL,'nv92.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1630,8 +1630,8 @@
       <c r="I10" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>192</v>
+      <c r="J10" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K10" s="3">
         <v>44993.412780362698</v>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('nv101','GD','GK',NULL,N'Ngữ văn lớp 10 tập 1',NULL,'nv101.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('nv101','GD','GK',NULL,N'Ngữ văn lớp 10 tập 1',NULL,'nv101.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1673,8 +1673,8 @@
       <c r="I11" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>192</v>
+      <c r="J11" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K11" s="3">
         <v>44993.412780362698</v>
@@ -1684,7 +1684,7 @@
       </c>
       <c r="M11" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('nv102','GD','GK',NULL,N'Ngữ văn lớp 10 tập 2',NULL,'nv102.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('nv102','GD','GK',NULL,N'Ngữ văn lớp 10 tập 2',NULL,'nv102.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1716,8 +1716,8 @@
       <c r="I12" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>192</v>
+      <c r="J12" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K12" s="3">
         <v>44993.412780362698</v>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="M12" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('nv111','GD','GK',NULL,N'Ngữ văn lớp 11 tập 1',NULL,'nv111.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('nv111','GD','GK',NULL,N'Ngữ văn lớp 11 tập 1',NULL,'nv111.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1759,8 +1759,8 @@
       <c r="I13" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>192</v>
+      <c r="J13" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K13" s="3">
         <v>44993.412780362698</v>
@@ -1770,7 +1770,7 @@
       </c>
       <c r="M13" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('nv112','GD','GK',NULL,N'Ngữ văn lớp 11 tập 2',NULL,'nv112.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('nv112','GD','GK',NULL,N'Ngữ văn lớp 11 tập 2',NULL,'nv112.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1802,8 +1802,8 @@
       <c r="I14" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>192</v>
+      <c r="J14" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K14" s="3">
         <v>44993.412780362698</v>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="M14" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('nv121','GD','GK',NULL,N'Ngữ văn lớp 12 tập 1',NULL,'nv121.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('nv121','GD','GK',NULL,N'Ngữ văn lớp 12 tập 1',NULL,'nv121.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1845,8 +1845,8 @@
       <c r="I15" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>192</v>
+      <c r="J15" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K15" s="3">
         <v>44993.412780362698</v>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="M15" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('nv122','GD','GK',NULL,N'Ngữ văn lớp 12 tập 2',NULL,'nv122.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('nv122','GD','GK',NULL,N'Ngữ văn lớp 12 tập 2',NULL,'nv122.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1888,8 +1888,8 @@
       <c r="I16" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>192</v>
+      <c r="J16" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K16" s="3">
         <v>44993.412780362698</v>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="M16" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('t61','GD','GK',NULL,N'Toán lớp 6 tập 1',NULL,'t61.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('t61','GD','GK',NULL,N'Toán lớp 6 tập 1',NULL,'t61.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1931,8 +1931,8 @@
       <c r="I17" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>192</v>
+      <c r="J17" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K17" s="3">
         <v>44993.412780362698</v>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="M17" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('t62','GD','GK',NULL,N'Toán lớp 6 tập 2',NULL,'t62.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('t62','GD','GK',NULL,N'Toán lớp 6 tập 2',NULL,'t62.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1974,8 +1974,8 @@
       <c r="I18" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>192</v>
+      <c r="J18" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K18" s="3">
         <v>44993.412780362698</v>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="M18" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('t71','GD','GK',NULL,N'Toán lớp 7 tập 1',NULL,'t71.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('t71','GD','GK',NULL,N'Toán lớp 7 tập 1',NULL,'t71.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2017,8 +2017,8 @@
       <c r="I19" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>192</v>
+      <c r="J19" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K19" s="3">
         <v>44993.412780362698</v>
@@ -2028,7 +2028,7 @@
       </c>
       <c r="M19" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('t72','GD','GK',NULL,N'Toán lớp 7 tập 2',NULL,'t72.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('t72','GD','GK',NULL,N'Toán lớp 7 tập 2',NULL,'t72.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2060,8 +2060,8 @@
       <c r="I20" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>192</v>
+      <c r="J20" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K20" s="3">
         <v>44993.412780362698</v>
@@ -2071,7 +2071,7 @@
       </c>
       <c r="M20" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('t81','GD','GK',NULL,N'Toán lớp 8 tập 1',NULL,'t81.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('t81','GD','GK',NULL,N'Toán lớp 8 tập 1',NULL,'t81.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -2103,8 +2103,8 @@
       <c r="I21" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>192</v>
+      <c r="J21" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K21" s="3">
         <v>44993.412780362698</v>
@@ -2114,7 +2114,7 @@
       </c>
       <c r="M21" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('t82','GD','GK',NULL,N'Toán lớp 8 tập 2',NULL,'t82.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('t82','GD','GK',NULL,N'Toán lớp 8 tập 2',NULL,'t82.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2146,8 +2146,8 @@
       <c r="I22" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>192</v>
+      <c r="J22" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K22" s="3">
         <v>44993.412780362698</v>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="M22" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('t91','GD','GK',NULL,N'Toán lớp 9 tập 1',NULL,'t91.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('t91','GD','GK',NULL,N'Toán lớp 9 tập 1',NULL,'t91.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -2189,8 +2189,8 @@
       <c r="I23" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>192</v>
+      <c r="J23" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K23" s="3">
         <v>44993.412780362698</v>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="M23" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('t92','GD','GK',NULL,N'Toán lớp 9 tập 2',NULL,'t92.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('t92','GD','GK',NULL,N'Toán lớp 9 tập 2',NULL,'t92.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -2232,8 +2232,8 @@
       <c r="I24" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>192</v>
+      <c r="J24" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K24" s="3">
         <v>44993.412780362698</v>
@@ -2243,7 +2243,7 @@
       </c>
       <c r="M24" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('t-ds10','GD','GK',NULL,N'Toán đại số lớp 10',NULL,'t-ds10.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('t-ds10','GD','GK',NULL,N'Toán đại số lớp 10',NULL,'t-ds10.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2275,8 +2275,8 @@
       <c r="I25" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>192</v>
+      <c r="J25" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K25" s="3">
         <v>44993.412780362698</v>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="M25" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('t-ds11','GD','GK',NULL,N'Toán đại số lớp 11',NULL,'t-ds11.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('t-ds11','GD','GK',NULL,N'Toán đại số lớp 11',NULL,'t-ds11.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2318,8 +2318,8 @@
       <c r="I26" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>192</v>
+      <c r="J26" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K26" s="3">
         <v>44993.412780362698</v>
@@ -2329,7 +2329,7 @@
       </c>
       <c r="M26" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('t-ds12','GD','GK',NULL,N'Toán đại số lớp 12',NULL,'t-ds12.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('t-ds12','GD','GK',NULL,N'Toán đại số lớp 12',NULL,'t-ds12.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -2361,8 +2361,8 @@
       <c r="I27" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>192</v>
+      <c r="J27" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K27" s="3">
         <v>44993.412780362698</v>
@@ -2372,7 +2372,7 @@
       </c>
       <c r="M27" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('t-hh10','GD','GK',NULL,N'Toán hình học lớp 10',NULL,'t-hh10.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('t-hh10','GD','GK',NULL,N'Toán hình học lớp 10',NULL,'t-hh10.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -2404,8 +2404,8 @@
       <c r="I28" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>192</v>
+      <c r="J28" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K28" s="3">
         <v>44993.412780362698</v>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="M28" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('t-hh11','GD','GK',NULL,N'Toán hình học lớp 11',NULL,'t-hh11.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('t-hh11','GD','GK',NULL,N'Toán hình học lớp 11',NULL,'t-hh11.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -2447,8 +2447,8 @@
       <c r="I29" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J29" s="1" t="s">
-        <v>192</v>
+      <c r="J29" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K29" s="3">
         <v>44993.412780362698</v>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="M29" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('t-hh12','GD','GK',NULL,N'Toán hình học  lớp 12',NULL,'t-hh12.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('t-hh12','GD','GK',NULL,N'Toán hình học  lớp 12',NULL,'t-hh12.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2490,8 +2490,8 @@
       <c r="I30" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J30" s="1" t="s">
-        <v>192</v>
+      <c r="J30" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K30" s="3">
         <v>44993.412780362698</v>
@@ -2501,7 +2501,7 @@
       </c>
       <c r="M30" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('ta6','GD','GK',NULL,N'Tiếng anh lớp 6',NULL,'ta6.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ta6','GD','GK',NULL,N'Tiếng anh lớp 6',NULL,'ta6.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2533,8 +2533,8 @@
       <c r="I31" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>192</v>
+      <c r="J31" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K31" s="3">
         <v>44993.412780362698</v>
@@ -2544,7 +2544,7 @@
       </c>
       <c r="M31" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('ta7','GD','GK',NULL,N'Tiếng anh lớp 7',NULL,'ta7.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ta7','GD','GK',NULL,N'Tiếng anh lớp 7',NULL,'ta7.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2576,8 +2576,8 @@
       <c r="I32" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>192</v>
+      <c r="J32" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K32" s="3">
         <v>44993.412780362698</v>
@@ -2587,7 +2587,7 @@
       </c>
       <c r="M32" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('ta8','GD','GK',NULL,N'Tiếng anh lớp 8',NULL,'ta8.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ta8','GD','GK',NULL,N'Tiếng anh lớp 8',NULL,'ta8.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -2619,8 +2619,8 @@
       <c r="I33" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J33" s="1" t="s">
-        <v>192</v>
+      <c r="J33" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K33" s="3">
         <v>44993.412780362698</v>
@@ -2630,7 +2630,7 @@
       </c>
       <c r="M33" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('ta9','GD','GK',NULL,N'Tiếng anh lớp 9',NULL,'ta9.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ta9','GD','GK',NULL,N'Tiếng anh lớp 9',NULL,'ta9.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -2662,8 +2662,8 @@
       <c r="I34" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J34" s="1" t="s">
-        <v>192</v>
+      <c r="J34" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K34" s="3">
         <v>44993.412780362698</v>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="M34" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('ta10','GD','GK',NULL,N'Tiếng anh lớp 10',NULL,'ta10.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ta10','GD','GK',NULL,N'Tiếng anh lớp 10',NULL,'ta10.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2705,8 +2705,8 @@
       <c r="I35" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>192</v>
+      <c r="J35" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K35" s="3">
         <v>44993.412780362698</v>
@@ -2716,7 +2716,7 @@
       </c>
       <c r="M35" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('ta11','GD','GK',NULL,N'Tiếng anh lớp 11',NULL,'ta11.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ta11','GD','GK',NULL,N'Tiếng anh lớp 11',NULL,'ta11.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2748,8 +2748,8 @@
       <c r="I36" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J36" s="1" t="s">
-        <v>192</v>
+      <c r="J36" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K36" s="3">
         <v>44993.412780362698</v>
@@ -2759,7 +2759,7 @@
       </c>
       <c r="M36" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('ta12','GD','GK',NULL,N'Tiếng anh lớp 12',NULL,'ta12.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ta12','GD','GK',NULL,N'Tiếng anh lớp 12',NULL,'ta12.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2791,8 +2791,8 @@
       <c r="I37" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>192</v>
+      <c r="J37" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K37" s="3">
         <v>44993.412780362698</v>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="M37" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('h8','GD','GK',NULL,N'Hoá lớp 8',NULL,'h8.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('h8','GD','GK',NULL,N'Hoá lớp 8',NULL,'h8.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2834,8 +2834,8 @@
       <c r="I38" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>192</v>
+      <c r="J38" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K38" s="3">
         <v>44993.412780362698</v>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="M38" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('h9','GD','GK',NULL,N'Hoá lớp 9',NULL,'h9.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('h9','GD','GK',NULL,N'Hoá lớp 9',NULL,'h9.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2877,8 +2877,8 @@
       <c r="I39" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>192</v>
+      <c r="J39" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K39" s="3">
         <v>44993.412780362698</v>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="M39" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('h10','GD','GK',NULL,N'Hoá lớp 10',NULL,'h10.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('h10','GD','GK',NULL,N'Hoá lớp 10',NULL,'h10.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2920,8 +2920,8 @@
       <c r="I40" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J40" s="1" t="s">
-        <v>192</v>
+      <c r="J40" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K40" s="3">
         <v>44993.412780362698</v>
@@ -2931,7 +2931,7 @@
       </c>
       <c r="M40" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('h11','GD','GK',NULL,N'Hoá lớp 11',NULL,'h11.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('h11','GD','GK',NULL,N'Hoá lớp 11',NULL,'h11.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -2963,8 +2963,8 @@
       <c r="I41" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J41" s="1" t="s">
-        <v>192</v>
+      <c r="J41" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K41" s="3">
         <v>44993.412780362698</v>
@@ -2974,7 +2974,7 @@
       </c>
       <c r="M41" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('h12','GD','GK',NULL,N'Hoá lớp 12',NULL,'h12.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('h12','GD','GK',NULL,N'Hoá lớp 12',NULL,'h12.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -3006,8 +3006,8 @@
       <c r="I42" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J42" s="1" t="s">
-        <v>192</v>
+      <c r="J42" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K42" s="3">
         <v>44993.412780362698</v>
@@ -3017,7 +3017,7 @@
       </c>
       <c r="M42" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('l6','GD','GK',NULL,N'Vật lí lớp 6',NULL,'l6.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('l6','GD','GK',NULL,N'Vật lí lớp 6',NULL,'l6.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -3049,8 +3049,8 @@
       <c r="I43" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J43" s="1" t="s">
-        <v>192</v>
+      <c r="J43" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K43" s="3">
         <v>44993.412780362698</v>
@@ -3060,7 +3060,7 @@
       </c>
       <c r="M43" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('l7','GD','GK',NULL,N'Vật lí lớp 7',NULL,'l7.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('l7','GD','GK',NULL,N'Vật lí lớp 7',NULL,'l7.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -3092,8 +3092,8 @@
       <c r="I44" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>192</v>
+      <c r="J44" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K44" s="3">
         <v>44993.412780362698</v>
@@ -3103,7 +3103,7 @@
       </c>
       <c r="M44" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('l8','GD','GK',NULL,N'Vật lí lớp 8',NULL,'l8.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('l8','GD','GK',NULL,N'Vật lí lớp 8',NULL,'l8.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -3135,8 +3135,8 @@
       <c r="I45" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J45" s="1" t="s">
-        <v>192</v>
+      <c r="J45" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K45" s="3">
         <v>44993.412780362698</v>
@@ -3146,7 +3146,7 @@
       </c>
       <c r="M45" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('l9','GD','GK',NULL,N'Vật lí lớp 9',NULL,'l9.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('l9','GD','GK',NULL,N'Vật lí lớp 9',NULL,'l9.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -3178,8 +3178,8 @@
       <c r="I46" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J46" s="1" t="s">
-        <v>192</v>
+      <c r="J46" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K46" s="3">
         <v>44993.412780362698</v>
@@ -3189,7 +3189,7 @@
       </c>
       <c r="M46" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('l10','GD','GK',NULL,N'Vật lí lớp 10',NULL,'l10.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('l10','GD','GK',NULL,N'Vật lí lớp 10',NULL,'l10.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -3221,8 +3221,8 @@
       <c r="I47" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J47" s="1" t="s">
-        <v>192</v>
+      <c r="J47" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K47" s="3">
         <v>44993.412780362698</v>
@@ -3232,7 +3232,7 @@
       </c>
       <c r="M47" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('l11','GD','GK',NULL,N'Vật lí lớp 11',NULL,'l11.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('l11','GD','GK',NULL,N'Vật lí lớp 11',NULL,'l11.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -3264,8 +3264,8 @@
       <c r="I48" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J48" s="1" t="s">
-        <v>192</v>
+      <c r="J48" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K48" s="3">
         <v>44993.412780362698</v>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="M48" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('l12','GD','GK',NULL,N'Vật lí lớp 12',NULL,'l12.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('l12','GD','GK',NULL,N'Vật lí lớp 12',NULL,'l12.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -3307,8 +3307,8 @@
       <c r="I49" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J49" s="1" t="s">
-        <v>192</v>
+      <c r="J49" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K49" s="3">
         <v>44993.412780362698</v>
@@ -3318,7 +3318,7 @@
       </c>
       <c r="M49" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('cn6','GD','GK',NULL,N'Công nghệ lớp 6',NULL,'cn6.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('cn6','GD','GK',NULL,N'Công nghệ lớp 6',NULL,'cn6.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -3350,8 +3350,8 @@
       <c r="I50" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J50" s="1" t="s">
-        <v>192</v>
+      <c r="J50" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K50" s="3">
         <v>44993.412780362698</v>
@@ -3361,7 +3361,7 @@
       </c>
       <c r="M50" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('cn7','GD','GK',NULL,N'Công nghệ lớp 7',NULL,'cn7.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('cn7','GD','GK',NULL,N'Công nghệ lớp 7',NULL,'cn7.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -3393,8 +3393,8 @@
       <c r="I51" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J51" s="1" t="s">
-        <v>192</v>
+      <c r="J51" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K51" s="3">
         <v>44993.412780362698</v>
@@ -3404,7 +3404,7 @@
       </c>
       <c r="M51" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('cn8','GD','GK',NULL,N'Công nghệ lớp 8',NULL,'cn8.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('cn8','GD','GK',NULL,N'Công nghệ lớp 8',NULL,'cn8.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -3436,8 +3436,8 @@
       <c r="I52" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J52" s="1" t="s">
-        <v>192</v>
+      <c r="J52" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K52" s="3">
         <v>44993.412780362698</v>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="M52" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('cn9','GD','GK',NULL,N'Công nghệ lớp 9',NULL,'cn9.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('cn9','GD','GK',NULL,N'Công nghệ lớp 9',NULL,'cn9.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -3479,8 +3479,8 @@
       <c r="I53" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J53" s="1" t="s">
-        <v>192</v>
+      <c r="J53" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K53" s="3">
         <v>44993.412780362698</v>
@@ -3490,7 +3490,7 @@
       </c>
       <c r="M53" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('cn10','GD','GK',NULL,N'Công nghệ lớp 10',NULL,'cn10.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('cn10','GD','GK',NULL,N'Công nghệ lớp 10',NULL,'cn10.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -3522,8 +3522,8 @@
       <c r="I54" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J54" s="1" t="s">
-        <v>192</v>
+      <c r="J54" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K54" s="3">
         <v>44993.412780362698</v>
@@ -3533,7 +3533,7 @@
       </c>
       <c r="M54" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('cn11','GD','GK',NULL,N'Công nghệ lớp 11',NULL,'cn11.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('cn11','GD','GK',NULL,N'Công nghệ lớp 11',NULL,'cn11.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -3565,8 +3565,8 @@
       <c r="I55" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J55" s="1" t="s">
-        <v>192</v>
+      <c r="J55" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K55" s="3">
         <v>44993.412780362698</v>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="M55" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('cn12','GD','GK',NULL,N'Công nghệ lớp 12',NULL,'cn12.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('cn12','GD','GK',NULL,N'Công nghệ lớp 12',NULL,'cn12.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -3608,8 +3608,8 @@
       <c r="I56" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J56" s="1" t="s">
-        <v>192</v>
+      <c r="J56" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K56" s="3">
         <v>44993.412780362698</v>
@@ -3619,7 +3619,7 @@
       </c>
       <c r="M56" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('dl6','GD','GK',NULL,N'Địa lí lớp 6',NULL,'dl6.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('dl6','GD','GK',NULL,N'Địa lí lớp 6',NULL,'dl6.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -3651,8 +3651,8 @@
       <c r="I57" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J57" s="1" t="s">
-        <v>192</v>
+      <c r="J57" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K57" s="3">
         <v>44993.412780362698</v>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="M57" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('dl7','GD','GK',NULL,N'Địa lí lớp 7',NULL,'dl7.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('dl7','GD','GK',NULL,N'Địa lí lớp 7',NULL,'dl7.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -3694,8 +3694,8 @@
       <c r="I58" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J58" s="1" t="s">
-        <v>192</v>
+      <c r="J58" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K58" s="3">
         <v>44993.412780362698</v>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="M58" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('dl8','GD','GK',NULL,N'Địa lí lớp 8',NULL,'dl8.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('dl8','GD','GK',NULL,N'Địa lí lớp 8',NULL,'dl8.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -3737,8 +3737,8 @@
       <c r="I59" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J59" s="1" t="s">
-        <v>192</v>
+      <c r="J59" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K59" s="3">
         <v>44993.412780362698</v>
@@ -3748,7 +3748,7 @@
       </c>
       <c r="M59" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('dl9','GD','GK',NULL,N'Địa lí lớp 9',NULL,'dl9.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('dl9','GD','GK',NULL,N'Địa lí lớp 9',NULL,'dl9.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -3780,8 +3780,8 @@
       <c r="I60" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J60" s="1" t="s">
-        <v>192</v>
+      <c r="J60" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K60" s="3">
         <v>44993.412780362698</v>
@@ -3791,7 +3791,7 @@
       </c>
       <c r="M60" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('dl10','GD','GK',NULL,N'Địa lí lớp 10',NULL,'dl10.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('dl10','GD','GK',NULL,N'Địa lí lớp 10',NULL,'dl10.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -3823,8 +3823,8 @@
       <c r="I61" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J61" s="1" t="s">
-        <v>192</v>
+      <c r="J61" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K61" s="3">
         <v>44993.412780362698</v>
@@ -3834,7 +3834,7 @@
       </c>
       <c r="M61" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('dl11','GD','GK',NULL,N'Địa lí lớp 11',NULL,'dl11.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('dl11','GD','GK',NULL,N'Địa lí lớp 11',NULL,'dl11.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -3866,8 +3866,8 @@
       <c r="I62" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J62" s="1" t="s">
-        <v>192</v>
+      <c r="J62" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K62" s="3">
         <v>44993.412780362698</v>
@@ -3877,7 +3877,7 @@
       </c>
       <c r="M62" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('dl12','GD','GK',NULL,N'Địa lí lớp 12',NULL,'dl12.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('dl12','GD','GK',NULL,N'Địa lí lớp 12',NULL,'dl12.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -3909,8 +3909,8 @@
       <c r="I63" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J63" s="1" t="s">
-        <v>192</v>
+      <c r="J63" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K63" s="3">
         <v>44993.412780362698</v>
@@ -3920,7 +3920,7 @@
       </c>
       <c r="M63" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('ls6','GD','GK',NULL,N'Lịch sử lớp 6',NULL,'ls6.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ls6','GD','GK',NULL,N'Lịch sử lớp 6',NULL,'ls6.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -3952,8 +3952,8 @@
       <c r="I64" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J64" s="1" t="s">
-        <v>192</v>
+      <c r="J64" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K64" s="3">
         <v>44993.412780362698</v>
@@ -3963,7 +3963,7 @@
       </c>
       <c r="M64" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('ls7','GD','GK',NULL,N'Lịch sử lớp 7',NULL,'ls7.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ls7','GD','GK',NULL,N'Lịch sử lớp 7',NULL,'ls7.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -3995,8 +3995,8 @@
       <c r="I65" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J65" s="1" t="s">
-        <v>192</v>
+      <c r="J65" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K65" s="3">
         <v>44993.412780362698</v>
@@ -4006,7 +4006,7 @@
       </c>
       <c r="M65" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('ls8','GD','GK',NULL,N'Lịch sử lớp 8',NULL,'ls8.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ls8','GD','GK',NULL,N'Lịch sử lớp 8',NULL,'ls8.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -4038,8 +4038,8 @@
       <c r="I66" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J66" s="1" t="s">
-        <v>192</v>
+      <c r="J66" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K66" s="3">
         <v>44993.412780362698</v>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="M66" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Sach VALUES('ls9','GD','GK',NULL,N'Lịch sử lớp 9',NULL,'ls9.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ls9','GD','GK',NULL,N'Lịch sử lớp 9',NULL,'ls9.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -4081,8 +4081,8 @@
       <c r="I67" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J67" s="1" t="s">
-        <v>192</v>
+      <c r="J67" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K67" s="3">
         <v>44993.412780362698</v>
@@ -4092,7 +4092,7 @@
       </c>
       <c r="M67" t="str">
         <f t="shared" ref="M67:M126" si="3">"INSERT INTO Sach VALUES('"&amp;A67&amp;"','"&amp;B67&amp;"','"&amp;C67&amp;"',"&amp;D67&amp;",N'"&amp;E67&amp;"',"&amp;F67&amp;",'"&amp;G67&amp;"',"&amp;H67&amp;",1,"&amp;J67&amp;",'',"&amp;L67&amp;")"</f>
-        <v>INSERT INTO Sach VALUES('ls10','GD','GK',NULL,N'Lịch sử lớp 10',NULL,'ls10.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ls10','GD','GK',NULL,N'Lịch sử lớp 10',NULL,'ls10.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -4124,8 +4124,8 @@
       <c r="I68" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J68" s="1" t="s">
-        <v>192</v>
+      <c r="J68" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K68" s="3">
         <v>44993.412780362698</v>
@@ -4135,7 +4135,7 @@
       </c>
       <c r="M68" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('ls11','GD','GK',NULL,N'Lịch sử lớp 11',NULL,'ls11.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ls11','GD','GK',NULL,N'Lịch sử lớp 11',NULL,'ls11.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -4167,8 +4167,8 @@
       <c r="I69" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J69" s="1" t="s">
-        <v>192</v>
+      <c r="J69" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K69" s="3">
         <v>44993.412780362698</v>
@@ -4178,7 +4178,7 @@
       </c>
       <c r="M69" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('ls12','GD','GK',NULL,N'Lịch sử lớp 12',NULL,'ls12.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ls12','GD','GK',NULL,N'Lịch sử lớp 12',NULL,'ls12.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -4210,8 +4210,8 @@
       <c r="I70" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J70" s="1" t="s">
-        <v>192</v>
+      <c r="J70" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K70" s="3">
         <v>44993.412780362698</v>
@@ -4221,7 +4221,7 @@
       </c>
       <c r="M70" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('s6','GD','GK',NULL,N'Sinh học lớp 6',NULL,'s6.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('s6','GD','GK',NULL,N'Sinh học lớp 6',NULL,'s6.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -4253,8 +4253,8 @@
       <c r="I71" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J71" s="1" t="s">
-        <v>192</v>
+      <c r="J71" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K71" s="3">
         <v>44993.412780362698</v>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="M71" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('s7','GD','GK',NULL,N'Sinh học lớp 7',NULL,'s7.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('s7','GD','GK',NULL,N'Sinh học lớp 7',NULL,'s7.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -4296,8 +4296,8 @@
       <c r="I72" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J72" s="1" t="s">
-        <v>192</v>
+      <c r="J72" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K72" s="3">
         <v>44993.412780362698</v>
@@ -4307,7 +4307,7 @@
       </c>
       <c r="M72" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('s8','GD','GK',NULL,N'Sinh học lớp 8',NULL,'s8.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('s8','GD','GK',NULL,N'Sinh học lớp 8',NULL,'s8.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -4339,8 +4339,8 @@
       <c r="I73" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J73" s="1" t="s">
-        <v>192</v>
+      <c r="J73" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K73" s="3">
         <v>44993.412780362698</v>
@@ -4350,7 +4350,7 @@
       </c>
       <c r="M73" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('s9','GD','GK',NULL,N'Sinh học lớp 9',NULL,'s9.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('s9','GD','GK',NULL,N'Sinh học lớp 9',NULL,'s9.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -4382,8 +4382,8 @@
       <c r="I74" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J74" s="1" t="s">
-        <v>192</v>
+      <c r="J74" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K74" s="3">
         <v>44993.412780362698</v>
@@ -4393,7 +4393,7 @@
       </c>
       <c r="M74" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('s10','GD','GK',NULL,N'Sinh học lớp 10',NULL,'s10.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('s10','GD','GK',NULL,N'Sinh học lớp 10',NULL,'s10.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -4425,8 +4425,8 @@
       <c r="I75" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J75" s="1" t="s">
-        <v>192</v>
+      <c r="J75" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K75" s="3">
         <v>44993.412780362698</v>
@@ -4436,7 +4436,7 @@
       </c>
       <c r="M75" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('s11','GD','GK',NULL,N'Sinh học lớp 11',NULL,'s11.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('s11','GD','GK',NULL,N'Sinh học lớp 11',NULL,'s11.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -4468,8 +4468,8 @@
       <c r="I76" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J76" s="1" t="s">
-        <v>192</v>
+      <c r="J76" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K76" s="3">
         <v>44993.412780362698</v>
@@ -4479,7 +4479,7 @@
       </c>
       <c r="M76" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('s12','GD','GK',NULL,N'Sinh học lớp 12',NULL,'s12.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('s12','GD','GK',NULL,N'Sinh học lớp 12',NULL,'s12.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -4511,8 +4511,8 @@
       <c r="I77" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J77" s="1" t="s">
-        <v>192</v>
+      <c r="J77" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K77" s="3">
         <v>44993.412780362698</v>
@@ -4522,7 +4522,7 @@
       </c>
       <c r="M77" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('gdcd6','GD','GK',NULL,N'Giáo dục công dân lớp 6',NULL,'gdcd6.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('gdcd6','GD','GK',NULL,N'Giáo dục công dân lớp 6',NULL,'gdcd6.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -4554,8 +4554,8 @@
       <c r="I78" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J78" s="1" t="s">
-        <v>192</v>
+      <c r="J78" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K78" s="3">
         <v>44993.412780362698</v>
@@ -4565,7 +4565,7 @@
       </c>
       <c r="M78" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('gdcd7','GD','GK',NULL,N'Giáo dục công dân lớp 7',NULL,'gdcd7.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('gdcd7','GD','GK',NULL,N'Giáo dục công dân lớp 7',NULL,'gdcd7.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -4597,8 +4597,8 @@
       <c r="I79" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J79" s="1" t="s">
-        <v>192</v>
+      <c r="J79" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K79" s="3">
         <v>44993.412780362698</v>
@@ -4608,7 +4608,7 @@
       </c>
       <c r="M79" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('gdcd8','GD','GK',NULL,N'Giáo dục công dân lớp 8',NULL,'gdcd8.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('gdcd8','GD','GK',NULL,N'Giáo dục công dân lớp 8',NULL,'gdcd8.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -4640,8 +4640,8 @@
       <c r="I80" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J80" s="1" t="s">
-        <v>192</v>
+      <c r="J80" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K80" s="3">
         <v>44993.412780362698</v>
@@ -4651,7 +4651,7 @@
       </c>
       <c r="M80" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('gdcd9','GD','GK',NULL,N'Giáo dục công dân lớp 9',NULL,'gdcd9.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('gdcd9','GD','GK',NULL,N'Giáo dục công dân lớp 9',NULL,'gdcd9.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -4683,8 +4683,8 @@
       <c r="I81" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J81" s="1" t="s">
-        <v>192</v>
+      <c r="J81" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K81" s="3">
         <v>44993.412780362698</v>
@@ -4694,7 +4694,7 @@
       </c>
       <c r="M81" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('gdcd10','GD','GK',NULL,N'Giáo dục công dân lớp 10',NULL,'gdcd10.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('gdcd10','GD','GK',NULL,N'Giáo dục công dân lớp 10',NULL,'gdcd10.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -4726,8 +4726,8 @@
       <c r="I82" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J82" s="1" t="s">
-        <v>192</v>
+      <c r="J82" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K82" s="3">
         <v>44993.412780362698</v>
@@ -4737,7 +4737,7 @@
       </c>
       <c r="M82" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('gdcd11','GD','GK',NULL,N'Giáo dục công dân lớp 11',NULL,'gdcd11.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('gdcd11','GD','GK',NULL,N'Giáo dục công dân lớp 11',NULL,'gdcd11.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -4769,8 +4769,8 @@
       <c r="I83" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J83" s="1" t="s">
-        <v>192</v>
+      <c r="J83" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K83" s="3">
         <v>44993.412780362698</v>
@@ -4780,7 +4780,7 @@
       </c>
       <c r="M83" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('gdcd12','GD','GK',NULL,N'Giáo dục công dân lớp 12',NULL,'gdcd12.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('gdcd12','GD','GK',NULL,N'Giáo dục công dân lớp 12',NULL,'gdcd12.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -4812,8 +4812,8 @@
       <c r="I84" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J84" s="1" t="s">
-        <v>192</v>
+      <c r="J84" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K84" s="3">
         <v>44993.412780362698</v>
@@ -4823,7 +4823,7 @@
       </c>
       <c r="M84" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('gdqp10','GD','GK',NULL,N'Giáo dục quốc phòng lớp 10',NULL,'gdqp10.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('gdqp10','GD','GK',NULL,N'Giáo dục quốc phòng lớp 10',NULL,'gdqp10.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -4855,8 +4855,8 @@
       <c r="I85" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J85" s="1" t="s">
-        <v>192</v>
+      <c r="J85" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K85" s="3">
         <v>44993.412780362698</v>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="M85" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('gdqp11','GD','GK',NULL,N'Giáo dục quốc phòng lớp 11',NULL,'gdqp11.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('gdqp11','GD','GK',NULL,N'Giáo dục quốc phòng lớp 11',NULL,'gdqp11.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -4898,8 +4898,8 @@
       <c r="I86" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J86" s="1" t="s">
-        <v>192</v>
+      <c r="J86" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K86" s="3">
         <v>44993.412780362698</v>
@@ -4909,7 +4909,7 @@
       </c>
       <c r="M86" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('gdqp12','GD','GK',NULL,N'Giáo dục quốc phòng lớp 12',NULL,'gdqp12.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('gdqp12','GD','GK',NULL,N'Giáo dục quốc phòng lớp 12',NULL,'gdqp12.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
@@ -4941,8 +4941,8 @@
       <c r="I87" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J87" s="1" t="s">
-        <v>192</v>
+      <c r="J87" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K87" s="3">
         <v>44993.412780362698</v>
@@ -4952,7 +4952,7 @@
       </c>
       <c r="M87" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('an-v6','GD','GK',NULL,N'Âm nhạc và Mĩ thuật lớp 6',NULL,'an-v6.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('an-v6','GD','GK',NULL,N'Âm nhạc và Mĩ thuật lớp 6',NULL,'an-v6.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -4984,8 +4984,8 @@
       <c r="I88" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J88" s="1" t="s">
-        <v>192</v>
+      <c r="J88" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K88" s="3">
         <v>44993.412780362698</v>
@@ -4995,7 +4995,7 @@
       </c>
       <c r="M88" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('an-v7','GD','GK',NULL,N'Âm nhạc và Mĩ thuật lớp 7',NULL,'an-v7.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('an-v7','GD','GK',NULL,N'Âm nhạc và Mĩ thuật lớp 7',NULL,'an-v7.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -5027,8 +5027,8 @@
       <c r="I89" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J89" s="1" t="s">
-        <v>192</v>
+      <c r="J89" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K89" s="3">
         <v>44993.412780362698</v>
@@ -5038,7 +5038,7 @@
       </c>
       <c r="M89" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('an-v8','GD','GK',NULL,N'Âm nhạc và Mĩ thuật lớp 8',NULL,'an-v8.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('an-v8','GD','GK',NULL,N'Âm nhạc và Mĩ thuật lớp 8',NULL,'an-v8.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -5070,8 +5070,8 @@
       <c r="I90" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J90" s="1" t="s">
-        <v>192</v>
+      <c r="J90" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K90" s="3">
         <v>44993.412780362698</v>
@@ -5081,7 +5081,7 @@
       </c>
       <c r="M90" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('an-v9','GD','GK',NULL,N'Âm nhạc và Mĩ thuật lớp 9',NULL,'an-v9.jpg',5000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('an-v9','GD','GK',NULL,N'Âm nhạc và Mĩ thuật lớp 9',NULL,'an-v9.jpg',5000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -5116,8 +5116,8 @@
       <c r="I92" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J92" s="1" t="s">
-        <v>192</v>
+      <c r="J92" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K92" s="3">
         <v>44993.412780362698</v>
@@ -5127,7 +5127,7 @@
       </c>
       <c r="M92" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('kt-ta61','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 6 Tập 1',NULL,'kt-ta61.jpg',69000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('kt-ta61','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 6 Tập 1',NULL,'kt-ta61.jpg',69000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -5159,8 +5159,8 @@
       <c r="I93" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J93" s="1" t="s">
-        <v>192</v>
+      <c r="J93" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K93" s="3">
         <v>44993.412780362698</v>
@@ -5170,7 +5170,7 @@
       </c>
       <c r="M93" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('kt-ta62','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 6 Tập 2',NULL,'kt-ta62.jpg',69000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('kt-ta62','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 6 Tập 2',NULL,'kt-ta62.jpg',69000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
@@ -5202,8 +5202,8 @@
       <c r="I94" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J94" s="1" t="s">
-        <v>192</v>
+      <c r="J94" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K94" s="3">
         <v>44993.412780362698</v>
@@ -5213,7 +5213,7 @@
       </c>
       <c r="M94" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('kt-ta71','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 7 Tập 1',NULL,'kt-ta71.jpg',75000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('kt-ta71','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 7 Tập 1',NULL,'kt-ta71.jpg',75000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
@@ -5245,8 +5245,8 @@
       <c r="I95" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J95" s="1" t="s">
-        <v>192</v>
+      <c r="J95" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K95" s="3">
         <v>44993.412780362698</v>
@@ -5256,7 +5256,7 @@
       </c>
       <c r="M95" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('kt-ta72','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 7 Tập 2',NULL,'kt-ta72.jpg',75000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('kt-ta72','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 7 Tập 2',NULL,'kt-ta72.jpg',75000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
@@ -5288,8 +5288,8 @@
       <c r="I96" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J96" s="1" t="s">
-        <v>192</v>
+      <c r="J96" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K96" s="3">
         <v>44993.412780362698</v>
@@ -5299,7 +5299,7 @@
       </c>
       <c r="M96" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('kt-ta81','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 8 Tập 1',NULL,'kt-ta81.jpg',75000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('kt-ta81','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 8 Tập 1',NULL,'kt-ta81.jpg',75000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
@@ -5331,8 +5331,8 @@
       <c r="I97" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J97" s="1" t="s">
-        <v>192</v>
+      <c r="J97" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K97" s="3">
         <v>44993.412780362698</v>
@@ -5342,7 +5342,7 @@
       </c>
       <c r="M97" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('kt-ta82','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 8 Tập 2',NULL,'kt-ta82.jpg',75000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('kt-ta82','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 8 Tập 2',NULL,'kt-ta82.jpg',75000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -5374,8 +5374,8 @@
       <c r="I98" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J98" s="1" t="s">
-        <v>192</v>
+      <c r="J98" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K98" s="3">
         <v>44993.412780362698</v>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="M98" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('kt-ta91','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 9 Tập 1',NULL,'kt-ta91.jpg',85000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('kt-ta91','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 9 Tập 1',NULL,'kt-ta91.jpg',85000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -5417,8 +5417,8 @@
       <c r="I99" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J99" s="1" t="s">
-        <v>192</v>
+      <c r="J99" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K99" s="3">
         <v>44993.412780362698</v>
@@ -5428,7 +5428,7 @@
       </c>
       <c r="M99" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('kt-ta92','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 9 Tập 2',NULL,'kt-ta92.jpg',85000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('kt-ta92','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Tiếng Anh Lớp 9 Tập 2',NULL,'kt-ta92.jpg',85000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -5460,8 +5460,8 @@
       <c r="I100" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J100" s="1" t="s">
-        <v>192</v>
+      <c r="J100" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K100" s="3">
         <v>44993.412780362698</v>
@@ -5471,7 +5471,7 @@
       </c>
       <c r="M100" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('gd-ta10','DHQGHN','TK',NULL,N'Luyện Giải Bộ Đề Bồi Dưỡng Học Sinh Giỏi Tiếng Anh Lớp 10',NULL,'gd-ta10.jpg',90000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('gd-ta10','DHQGHN','TK',NULL,N'Luyện Giải Bộ Đề Bồi Dưỡng Học Sinh Giỏi Tiếng Anh Lớp 10',NULL,'gd-ta10.jpg',90000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
@@ -5503,8 +5503,8 @@
       <c r="I101" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J101" s="1" t="s">
-        <v>192</v>
+      <c r="J101" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K101" s="3">
         <v>44993.412780362698</v>
@@ -5514,7 +5514,7 @@
       </c>
       <c r="M101" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('gd-ta11','DHQGHN','TK',NULL,N'Luyện Giải Bộ Đề Bồi Dưỡng Học Sinh Giỏi Tiếng Anh Lớp 11',NULL,'gd-ta11.jpg',90000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('gd-ta11','DHQGHN','TK',NULL,N'Luyện Giải Bộ Đề Bồi Dưỡng Học Sinh Giỏi Tiếng Anh Lớp 11',NULL,'gd-ta11.jpg',90000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
@@ -5546,8 +5546,8 @@
       <c r="I102" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J102" s="1" t="s">
-        <v>192</v>
+      <c r="J102" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K102" s="3">
         <v>44993.412780362698</v>
@@ -5557,7 +5557,7 @@
       </c>
       <c r="M102" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('gd-ta12','DHQGHN','TK',NULL,N'Luyện Giải Bộ Đề Bồi Dưỡng Học Sinh Giỏi Tiếng Anh Lớp 12',NULL,'gd-ta12.jpg',90000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('gd-ta12','DHQGHN','TK',NULL,N'Luyện Giải Bộ Đề Bồi Dưỡng Học Sinh Giỏi Tiếng Anh Lớp 12',NULL,'gd-ta12.jpg',90000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
@@ -5589,8 +5589,8 @@
       <c r="I103" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J103" s="1" t="s">
-        <v>192</v>
+      <c r="J103" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K103" s="3">
         <v>44993.412780362698</v>
@@ -5600,7 +5600,7 @@
       </c>
       <c r="M103" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('ktdgnl-t6','DHQGHN','TK',NULL,N'Ôn Tập Kiểm Tra Đánh Giá Năng Lực Môn Toán Lớp 6',NULL,'ktdgnl-t6.jpg',63000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ktdgnl-t6','DHQGHN','TK',NULL,N'Ôn Tập Kiểm Tra Đánh Giá Năng Lực Môn Toán Lớp 6',NULL,'ktdgnl-t6.jpg',63000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
@@ -5632,8 +5632,8 @@
       <c r="I104" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J104" s="1" t="s">
-        <v>192</v>
+      <c r="J104" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K104" s="3">
         <v>44993.412780362698</v>
@@ -5643,7 +5643,7 @@
       </c>
       <c r="M104" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('kt-t6','DN','TK',NULL,N'60 Đề Kiểm Tra Toán 6 (Theo Chương Trình Giáo Dục Phổ Thông Mới)',NULL,'kt-t6.jpg',65000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('kt-t6','DN','TK',NULL,N'60 Đề Kiểm Tra Toán 6 (Theo Chương Trình Giáo Dục Phổ Thông Mới)',NULL,'kt-t6.jpg',65000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
@@ -5675,8 +5675,8 @@
       <c r="I105" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J105" s="1" t="s">
-        <v>192</v>
+      <c r="J105" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K105" s="3">
         <v>44993.412780362698</v>
@@ -5686,7 +5686,7 @@
       </c>
       <c r="M105" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('ppg-t71','DHQGHN','TK',NULL,N'Hướng Dẫn Học &amp; Phương Pháp Giải Toán Lớp 7 - Tập 1 (Bám Sát SGK Chân Trời Sáng Tạo)',NULL,'ppg-t71.jpg',65000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ppg-t71','DHQGHN','TK',NULL,N'Hướng Dẫn Học &amp; Phương Pháp Giải Toán Lớp 7 - Tập 1 (Bám Sát SGK Chân Trời Sáng Tạo)',NULL,'ppg-t71.jpg',65000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
@@ -5718,8 +5718,8 @@
       <c r="I106" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J106" s="1" t="s">
-        <v>192</v>
+      <c r="J106" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K106" s="3">
         <v>44993.412780362698</v>
@@ -5729,7 +5729,7 @@
       </c>
       <c r="M106" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('ppg-t72','DHQGHN','TK',NULL,N'Hướng Dẫn Học &amp; Phương Pháp Giải Toán Lớp 7 - Tập 2 (Bám Sát SGK Chân Trời Sáng Tạo)',NULL,'ppg-t72.jpg',65000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ppg-t72','DHQGHN','TK',NULL,N'Hướng Dẫn Học &amp; Phương Pháp Giải Toán Lớp 7 - Tập 2 (Bám Sát SGK Chân Trời Sáng Tạo)',NULL,'ppg-t72.jpg',65000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
@@ -5761,8 +5761,8 @@
       <c r="I107" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J107" s="1" t="s">
-        <v>192</v>
+      <c r="J107" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K107" s="3">
         <v>44993.412780362698</v>
@@ -5772,7 +5772,7 @@
       </c>
       <c r="M107" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('kt-t7','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Toán 7 (Bám Sát SGK Chân Trời Sáng Tạo)',NULL,'kt-t7.jpg',55000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('kt-t7','DHQGHN','TK',NULL,N'Bộ Đề Kiểm Tra Toán 7 (Bám Sát SGK Chân Trời Sáng Tạo)',NULL,'kt-t7.jpg',55000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
@@ -5804,8 +5804,8 @@
       <c r="I108" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J108" s="1" t="s">
-        <v>192</v>
+      <c r="J108" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K108" s="3">
         <v>44993.412780362698</v>
@@ -5815,7 +5815,7 @@
       </c>
       <c r="M108" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('100kt-t8','THTPHCM','TK',NULL,N'100 Đề Kiểm Tra Toán 8',NULL,'100kt-t8.jpg',80000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('100kt-t8','THTPHCM','TK',NULL,N'100 Đề Kiểm Tra Toán 8',NULL,'100kt-t8.jpg',80000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
@@ -5847,8 +5847,8 @@
       <c r="I109" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J109" s="1" t="s">
-        <v>192</v>
+      <c r="J109" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K109" s="3">
         <v>44993.412780362698</v>
@@ -5858,7 +5858,7 @@
       </c>
       <c r="M109" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('kt-t8','DN','TK',NULL,N'Đề Kiểm Tra Định Kì Toán 8',NULL,'kt-t8.jpg',43000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('kt-t8','DN','TK',NULL,N'Đề Kiểm Tra Định Kì Toán 8',NULL,'kt-t8.jpg',43000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
@@ -5890,8 +5890,8 @@
       <c r="I110" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J110" s="1" t="s">
-        <v>192</v>
+      <c r="J110" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K110" s="3">
         <v>44993.412780362698</v>
@@ -5901,7 +5901,7 @@
       </c>
       <c r="M110" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('kt-t8-1','DHQGHN','TK',NULL,N'Bộ Đề Kiểm tra Toán 8',NULL,'kt-t8-1.jpg',90000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('kt-t8-1','DHQGHN','TK',NULL,N'Bộ Đề Kiểm tra Toán 8',NULL,'kt-t8-1.jpg',90000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
@@ -5933,8 +5933,8 @@
       <c r="I111" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J111" s="1" t="s">
-        <v>192</v>
+      <c r="J111" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K111" s="3">
         <v>44993.412780362698</v>
@@ -5944,7 +5944,7 @@
       </c>
       <c r="M111" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('kttt-t9','TN','TK',NULL,N'Bộ Đề Kiểm Tra Môn Toán 9 Theo Hướng Thực Tế, Tích Hợp',NULL,'kttt-t9.jpg',100000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('kttt-t9','TN','TK',NULL,N'Bộ Đề Kiểm Tra Môn Toán 9 Theo Hướng Thực Tế, Tích Hợp',NULL,'kttt-t9.jpg',100000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
@@ -5976,8 +5976,8 @@
       <c r="I112" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J112" s="1" t="s">
-        <v>192</v>
+      <c r="J112" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K112" s="3">
         <v>44993.412780362698</v>
@@ -5987,7 +5987,7 @@
       </c>
       <c r="M112" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('dotcc-t9','DN','TK',NULL,N'Bộ Đề Ôn Thi Môn Toán 9 Vào Lớp 10',NULL,'dotcc-t9.jpg',51000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('dotcc-t9','DN','TK',NULL,N'Bộ Đề Ôn Thi Môn Toán 9 Vào Lớp 10',NULL,'dotcc-t9.jpg',51000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
@@ -6019,8 +6019,8 @@
       <c r="I113" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J113" s="1" t="s">
-        <v>192</v>
+      <c r="J113" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K113" s="3">
         <v>44993.412780362698</v>
@@ -6030,7 +6030,7 @@
       </c>
       <c r="M113" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('cp-ltl10-t9','DHQGHN','TK',NULL,N'Chinh Phục Luyện Thi Vào Lớp 10 Môn Toán Theo Chủ Đề',NULL,'cp-ltl10-t9.jpg',135000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('cp-ltl10-t9','DHQGHN','TK',NULL,N'Chinh Phục Luyện Thi Vào Lớp 10 Môn Toán Theo Chủ Đề',NULL,'cp-ltl10-t9.jpg',135000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
@@ -6062,8 +6062,8 @@
       <c r="I114" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J114" s="1" t="s">
-        <v>192</v>
+      <c r="J114" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K114" s="3">
         <v>44993.412780362698</v>
@@ -6073,7 +6073,7 @@
       </c>
       <c r="M114" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('std-lthsg-t9','THTPHCM','TK',NULL,N'Siêu Tư Duy Luyện Đề Chuẩn Bị Kỳ Thi HSG Toán Lớp 9',NULL,'std-lthsg-t9.jpg',126000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('std-lthsg-t9','THTPHCM','TK',NULL,N'Siêu Tư Duy Luyện Đề Chuẩn Bị Kỳ Thi HSG Toán Lớp 9',NULL,'std-lthsg-t9.jpg',126000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
@@ -6105,8 +6105,8 @@
       <c r="I115" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J115" s="1" t="s">
-        <v>192</v>
+      <c r="J115" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K115" s="3">
         <v>44993.412780362698</v>
@@ -6116,7 +6116,7 @@
       </c>
       <c r="M115" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('tk-t101','DHQGHN','TK',NULL,N'Sách Tham Khảo Toán 10 - Quyển 1 (Biên Soạn Theo Chương Trình GDPT Mới)',NULL,'tk-t101.jpg',90000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('tk-t101','DHQGHN','TK',NULL,N'Sách Tham Khảo Toán 10 - Quyển 1 (Biên Soạn Theo Chương Trình GDPT Mới)',NULL,'tk-t101.jpg',90000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
@@ -6148,8 +6148,8 @@
       <c r="I116" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J116" s="1" t="s">
-        <v>192</v>
+      <c r="J116" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K116" s="3">
         <v>44993.412780362698</v>
@@ -6159,7 +6159,7 @@
       </c>
       <c r="M116" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('tk-t102','DHQGHN','TK',NULL,N'Sách Tham Khảo Toán 10 - Quyển 2 (Biên Soạn Theo Chương Trình GDPT Mới)',NULL,'tk-t102.jpg',100000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('tk-t102','DHQGHN','TK',NULL,N'Sách Tham Khảo Toán 10 - Quyển 2 (Biên Soạn Theo Chương Trình GDPT Mới)',NULL,'tk-t102.jpg',100000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
@@ -6191,8 +6191,8 @@
       <c r="I117" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J117" s="1" t="s">
-        <v>192</v>
+      <c r="J117" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K117" s="3">
         <v>44993.412780362698</v>
@@ -6202,7 +6202,7 @@
       </c>
       <c r="M117" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('bd-th-t10','DHQGHN','TK',NULL,N'Bồi Dưỡng Năng Lực Tự Học Toán 10',NULL,'bd-th-t10.jpg',112000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('bd-th-t10','DHQGHN','TK',NULL,N'Bồi Dưỡng Năng Lực Tự Học Toán 10',NULL,'bd-th-t10.jpg',112000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
@@ -6234,8 +6234,8 @@
       <c r="I118" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J118" s="1" t="s">
-        <v>192</v>
+      <c r="J118" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K118" s="3">
         <v>44993.412780362698</v>
@@ -6245,7 +6245,7 @@
       </c>
       <c r="M118" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('ppg-hh10','DN','TK',NULL,N'Phân Loại Và Phương Pháp Giải Các Dạng Toán Hình Học 10 (Cơ Bản &amp; Nâng Cao)',NULL,'ppg-hh10.jpg',40000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ppg-hh10','DN','TK',NULL,N'Phân Loại Và Phương Pháp Giải Các Dạng Toán Hình Học 10 (Cơ Bản &amp; Nâng Cao)',NULL,'ppg-hh10.jpg',40000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
@@ -6277,8 +6277,8 @@
       <c r="I119" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J119" s="1" t="s">
-        <v>192</v>
+      <c r="J119" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K119" s="3">
         <v>44993.412780362698</v>
@@ -6288,7 +6288,7 @@
       </c>
       <c r="M119" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('ppg-ds11','DHQGHN','TK',NULL,N'Phương Pháp Giải Các Chuyên Đề Căn Bản Đại Số - Giải Tích 11',NULL,'ppg-ds11.jpg',97000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ppg-ds11','DHQGHN','TK',NULL,N'Phương Pháp Giải Các Chuyên Đề Căn Bản Đại Số - Giải Tích 11',NULL,'ppg-ds11.jpg',97000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
@@ -6320,8 +6320,8 @@
       <c r="I120" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J120" s="1" t="s">
-        <v>192</v>
+      <c r="J120" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K120" s="3">
         <v>44993.412780362698</v>
@@ -6331,7 +6331,7 @@
       </c>
       <c r="M120" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('ppg-hh11','DHQGHN','TK',NULL,N'Phân Dạng &amp; Phương pháp Giải Các Dạng Bài Tập Trắc Nghiệm - Hình Học 11',NULL,'ppg-hh11.jpg',56000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ppg-hh11','DHQGHN','TK',NULL,N'Phân Dạng &amp; Phương pháp Giải Các Dạng Bài Tập Trắc Nghiệm - Hình Học 11',NULL,'ppg-hh11.jpg',56000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
@@ -6363,8 +6363,8 @@
       <c r="I121" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J121" s="1" t="s">
-        <v>192</v>
+      <c r="J121" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K121" s="3">
         <v>44993.412780362698</v>
@@ -6374,7 +6374,7 @@
       </c>
       <c r="M121" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('tn-t11','DHQGHN','TK',NULL,N'Trắc Nghiệm Chuyên Đề Đại Số - Giải Tích &amp; Hình Học 11',NULL,'tn-t11.jpg',106000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('tn-t11','DHQGHN','TK',NULL,N'Trắc Nghiệm Chuyên Đề Đại Số - Giải Tích &amp; Hình Học 11',NULL,'tn-t11.jpg',106000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
@@ -6406,8 +6406,8 @@
       <c r="I122" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J122" s="1" t="s">
-        <v>192</v>
+      <c r="J122" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K122" s="3">
         <v>44993.412780362698</v>
@@ -6417,7 +6417,7 @@
       </c>
       <c r="M122" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('vdu-nc-t11','DHQGHN','TK',NULL,N'15 Chủ Đề Vận Dụng &amp; Nâng Cao Toán Trắc Nghiệm 11',NULL,'vdu-nc-t11.jpg',70000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('vdu-nc-t11','DHQGHN','TK',NULL,N'15 Chủ Đề Vận Dụng &amp; Nâng Cao Toán Trắc Nghiệm 11',NULL,'vdu-nc-t11.jpg',70000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
@@ -6449,8 +6449,8 @@
       <c r="I123" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J123" s="1" t="s">
-        <v>192</v>
+      <c r="J123" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K123" s="3">
         <v>44993.412780362698</v>
@@ -6460,7 +6460,7 @@
       </c>
       <c r="M123" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('tn-cd-t12','DHQGHN','TK',NULL,N'Trắc Nghiệm Chuyên Đề Giải Tích Và Hình Học 12',NULL,'tn-cd-t12.jpg',200000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('tn-cd-t12','DHQGHN','TK',NULL,N'Trắc Nghiệm Chuyên Đề Giải Tích Và Hình Học 12',NULL,'tn-cd-t12.jpg',200000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
@@ -6492,8 +6492,8 @@
       <c r="I124" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J124" s="1" t="s">
-        <v>192</v>
+      <c r="J124" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K124" s="3">
         <v>44993.412780362698</v>
@@ -6503,7 +6503,7 @@
       </c>
       <c r="M124" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('50dmh-t12','TN','TK',NULL,N'50 Đề Minh Họa 2023 Môn Toán Học',NULL,'50dmh-t12.jpg',180000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('50dmh-t12','TN','TK',NULL,N'50 Đề Minh Họa 2023 Môn Toán Học',NULL,'50dmh-t12.jpg',180000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
@@ -6535,8 +6535,8 @@
       <c r="I125" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J125" s="1" t="s">
-        <v>192</v>
+      <c r="J125" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K125" s="3">
         <v>44993.412777777776</v>
@@ -6546,7 +6546,7 @@
       </c>
       <c r="M125" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('ppg-ds12','DHQGHN','TK',NULL,N'Phương Pháp Giải Toán Chuyên Đề Giải Tích 12',NULL,'ppg-ds12.jpg',114000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('ppg-ds12','DHQGHN','TK',NULL,N'Phương Pháp Giải Toán Chuyên Đề Giải Tích 12',NULL,'ppg-ds12.jpg',114000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
@@ -6578,8 +6578,8 @@
       <c r="I126" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J126" s="1" t="s">
-        <v>192</v>
+      <c r="J126" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="K126" s="3">
         <v>44993.412777777776</v>
@@ -6589,7 +6589,7 @@
       </c>
       <c r="M126" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO Sach VALUES('o-t12','DN','TK',NULL,N'Tổng Ôn Toán Học (Tái Bản 2023)',NULL,'o-t12.jpg',180000,1,NULL,'',NULL)</v>
+        <v>INSERT INTO Sach VALUES('o-t12','DN','TK',NULL,N'Tổng Ôn Toán Học (Tái Bản 2023)',NULL,'o-t12.jpg',180000,1,FALSE,'',NULL)</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>